<commit_message>
added health regime analysis
</commit_message>
<xml_diff>
--- a/background info/DSM501A ratio to mg-m3.xlsx
+++ b/background info/DSM501A ratio to mg-m3.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4635" firstSheet="4" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4635" firstSheet="2" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="pcs per 0.01ft3" sheetId="2" r:id="rId1"/>
@@ -19,12 +19,41 @@
     <sheet name="limits for exposure" sheetId="5" r:id="rId5"/>
     <sheet name="Low P1 ratio to counts" sheetId="6" r:id="rId6"/>
   </sheets>
+  <definedNames>
+    <definedName name="solver_adj" localSheetId="4" hidden="1">'limits for exposure'!$B$7</definedName>
+    <definedName name="solver_cvg" localSheetId="4" hidden="1">0.0001</definedName>
+    <definedName name="solver_drv" localSheetId="4" hidden="1">1</definedName>
+    <definedName name="solver_eng" localSheetId="4" hidden="1">1</definedName>
+    <definedName name="solver_est" localSheetId="4" hidden="1">1</definedName>
+    <definedName name="solver_itr" localSheetId="4" hidden="1">2147483647</definedName>
+    <definedName name="solver_mip" localSheetId="4" hidden="1">2147483647</definedName>
+    <definedName name="solver_mni" localSheetId="4" hidden="1">30</definedName>
+    <definedName name="solver_mrt" localSheetId="4" hidden="1">0.075</definedName>
+    <definedName name="solver_msl" localSheetId="4" hidden="1">2</definedName>
+    <definedName name="solver_neg" localSheetId="4" hidden="1">1</definedName>
+    <definedName name="solver_nod" localSheetId="4" hidden="1">2147483647</definedName>
+    <definedName name="solver_num" localSheetId="4" hidden="1">0</definedName>
+    <definedName name="solver_nwt" localSheetId="4" hidden="1">1</definedName>
+    <definedName name="solver_opt" localSheetId="4" hidden="1">'limits for exposure'!$D$7</definedName>
+    <definedName name="solver_pre" localSheetId="4" hidden="1">0.000001</definedName>
+    <definedName name="solver_rbv" localSheetId="4" hidden="1">1</definedName>
+    <definedName name="solver_rlx" localSheetId="4" hidden="1">2</definedName>
+    <definedName name="solver_rsd" localSheetId="4" hidden="1">0</definedName>
+    <definedName name="solver_scl" localSheetId="4" hidden="1">1</definedName>
+    <definedName name="solver_sho" localSheetId="4" hidden="1">2</definedName>
+    <definedName name="solver_ssz" localSheetId="4" hidden="1">100</definedName>
+    <definedName name="solver_tim" localSheetId="4" hidden="1">2147483647</definedName>
+    <definedName name="solver_tol" localSheetId="4" hidden="1">0.01</definedName>
+    <definedName name="solver_typ" localSheetId="4" hidden="1">3</definedName>
+    <definedName name="solver_val" localSheetId="4" hidden="1">350</definedName>
+    <definedName name="solver_ver" localSheetId="4" hidden="1">3</definedName>
+  </definedNames>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="55">
   <si>
     <t>mg/m3</t>
   </si>
@@ -180,13 +209,22 @@
   </si>
   <si>
     <t>converted to 1 um with 4.29 factor</t>
+  </si>
+  <si>
+    <t>1 um counts per 0.01 ft3 converted to EPA scale</t>
+  </si>
+  <si>
+    <t>4E-16x4 – 2E-11x3 + 3E-07x2 + 0.0014x + 1.9915</t>
+  </si>
+  <si>
+    <t>converts hundreds of particles per ft3 to ug/m3, which is the same as particles per 0.01 ft3 output by shinyei</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -317,6 +355,14 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -619,7 +665,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="42">
+  <cellStyleXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
@@ -662,11 +708,18 @@
     <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="42"/>
   </cellXfs>
-  <cellStyles count="42">
+  <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
     <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
     <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
@@ -700,6 +753,7 @@
     <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
     <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
     <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Hyperlink" xfId="42" builtinId="8"/>
     <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
     <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
     <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
@@ -738,6 +792,7 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -824,6 +879,7 @@
             <c:dispRSqr val="1"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
+              <c:layout/>
               <c:numFmt formatCode="General" sourceLinked="0"/>
               <c:spPr>
                 <a:noFill/>
@@ -906,11 +962,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1424497216"/>
-        <c:axId val="1424498848"/>
+        <c:axId val="-72300208"/>
+        <c:axId val="-72299664"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="1424497216"/>
+        <c:axId val="-72300208"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -967,12 +1023,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1424498848"/>
+        <c:crossAx val="-72299664"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1424498848"/>
+        <c:axId val="-72299664"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1029,7 +1085,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1424497216"/>
+        <c:crossAx val="-72300208"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1093,6 +1149,7 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1178,6 +1235,7 @@
             <c:dispRSqr val="1"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
+              <c:layout/>
               <c:numFmt formatCode="General" sourceLinked="0"/>
               <c:spPr>
                 <a:noFill/>
@@ -1284,11 +1342,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1301444080"/>
-        <c:axId val="1301439184"/>
+        <c:axId val="-72297488"/>
+        <c:axId val="-72295856"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="1301444080"/>
+        <c:axId val="-72297488"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1345,12 +1403,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1301439184"/>
+        <c:crossAx val="-72295856"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1301439184"/>
+        <c:axId val="-72295856"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1407,7 +1465,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1301444080"/>
+        <c:crossAx val="-72297488"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1654,11 +1712,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1301430480"/>
-        <c:axId val="1301437008"/>
+        <c:axId val="-72308368"/>
+        <c:axId val="-72307824"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="1301430480"/>
+        <c:axId val="-72308368"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1715,12 +1773,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1301437008"/>
+        <c:crossAx val="-72307824"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1301437008"/>
+        <c:axId val="-72307824"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1777,7 +1835,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1301430480"/>
+        <c:crossAx val="-72308368"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4241,7 +4299,7 @@
   <dimension ref="A1:B16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="A2" sqref="A1:A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4310,10 +4368,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G41"/>
+  <dimension ref="A1:G47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4321,6 +4379,7 @@
     <col min="1" max="1" width="20.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="39.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
@@ -4405,418 +4464,490 @@
         <v>7.0696250000000003</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>23</v>
-      </c>
-      <c r="B7">
-        <v>5000</v>
-      </c>
-      <c r="D7">
-        <f>B7*4.28/100</f>
-        <v>214</v>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F6" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B7" s="2">
+        <v>41976.603670590026</v>
+      </c>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2">
+        <f>0.0000000000000004*B7^4-0.00000000002*B7^3+0.0000003*B7^2+0.0014*B7</f>
+        <v>350.00000715369953</v>
       </c>
       <c r="F7" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>21</v>
-      </c>
-      <c r="B8">
-        <v>1000</v>
-      </c>
-      <c r="D8">
-        <f>B8*4.28/100</f>
-        <v>42.8</v>
-      </c>
-      <c r="F8">
-        <f>4.29*B8</f>
-        <v>4290</v>
+      <c r="B8" s="2">
+        <v>39003.640760662413</v>
+      </c>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2">
+        <f t="shared" ref="D8:E19" si="1">0.0000000000000004*B8^4-0.00000000002*B8^3+0.0000003*B8^2+0.0014*B8</f>
+        <v>250.00000244527078</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9" s="2">
+        <v>34452.217498360711</v>
+      </c>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2">
+        <f t="shared" si="1"/>
+        <v>149.99999975382784</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B10" s="2">
+        <v>21304.581815529178</v>
+      </c>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2">
+        <f t="shared" si="1"/>
+        <v>54.999998389599696</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B11" s="2">
+        <v>12470.543843263693</v>
+      </c>
+      <c r="C11" s="2"/>
+      <c r="D11" s="2">
+        <f t="shared" si="1"/>
+        <v>35.0000011100622</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B12" s="2">
+        <v>4919.2264814302798</v>
+      </c>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2">
+        <f t="shared" si="1"/>
+        <v>11.999999895086336</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>23</v>
+      </c>
+      <c r="D13" s="2"/>
+      <c r="F13" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>21</v>
+      </c>
+      <c r="B14">
+        <v>1000</v>
+      </c>
+      <c r="D14" s="3">
+        <f t="shared" si="1"/>
+        <v>1.6803999999999999</v>
+      </c>
+      <c r="F14">
+        <f>4.29*B14</f>
+        <v>4290</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
         <v>20</v>
       </c>
-      <c r="B9">
+      <c r="B15">
         <v>350</v>
       </c>
-      <c r="C9">
+      <c r="C15">
         <v>1000</v>
       </c>
-      <c r="D9">
-        <f t="shared" ref="D9:E13" si="1">B9*4.28/100</f>
-        <v>14.98</v>
-      </c>
-      <c r="E9">
+      <c r="D15" s="3">
         <f t="shared" si="1"/>
-        <v>42.8</v>
-      </c>
-      <c r="F9">
-        <f t="shared" ref="F9:F13" si="2">4.29*B9</f>
+        <v>0.52589850250000003</v>
+      </c>
+      <c r="E15" s="3">
+        <f t="shared" si="1"/>
+        <v>1.6803999999999999</v>
+      </c>
+      <c r="F15">
+        <f t="shared" ref="F15:F19" si="2">4.29*B15</f>
         <v>1501.5</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
         <v>19</v>
       </c>
-      <c r="B10">
+      <c r="B16">
         <v>100</v>
       </c>
-      <c r="C10">
+      <c r="C16">
         <v>350</v>
       </c>
-      <c r="D10">
+      <c r="D16" s="3">
         <f t="shared" si="1"/>
-        <v>4.28</v>
-      </c>
-      <c r="E10">
+        <v>0.14298003999999997</v>
+      </c>
+      <c r="E16" s="3">
         <f t="shared" si="1"/>
-        <v>14.98</v>
-      </c>
-      <c r="F10">
+        <v>0.52589850250000003</v>
+      </c>
+      <c r="F16">
         <f t="shared" si="2"/>
         <v>429</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
         <v>22</v>
       </c>
-      <c r="B11">
+      <c r="B17">
         <v>50</v>
       </c>
-      <c r="C11">
+      <c r="C17">
         <v>100</v>
       </c>
-      <c r="D11">
+      <c r="D17" s="3">
         <f t="shared" si="1"/>
-        <v>2.14</v>
-      </c>
-      <c r="E11">
+        <v>7.074750249999999E-2</v>
+      </c>
+      <c r="E17" s="3">
         <f t="shared" si="1"/>
-        <v>4.28</v>
-      </c>
-      <c r="F11">
+        <v>0.14298003999999997</v>
+      </c>
+      <c r="F17">
         <f t="shared" si="2"/>
         <v>214.5</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
         <v>30</v>
       </c>
-      <c r="B12">
+      <c r="B18">
         <v>25</v>
       </c>
-      <c r="C12">
+      <c r="C18">
         <v>50</v>
       </c>
-      <c r="D12">
+      <c r="D18" s="3">
         <f t="shared" si="1"/>
-        <v>1.07</v>
-      </c>
-      <c r="E12">
+        <v>3.5187187656249994E-2</v>
+      </c>
+      <c r="E18" s="3">
         <f t="shared" si="1"/>
-        <v>2.14</v>
-      </c>
-      <c r="F12">
+        <v>7.074750249999999E-2</v>
+      </c>
+      <c r="F18">
         <f t="shared" si="2"/>
         <v>107.25</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
         <v>31</v>
       </c>
-      <c r="B13">
+      <c r="B19">
         <v>0</v>
       </c>
-      <c r="C13">
+      <c r="C19">
         <v>25</v>
       </c>
-      <c r="D13">
+      <c r="D19" s="3">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="E13">
+      <c r="E19" s="3">
         <f t="shared" si="1"/>
-        <v>1.07</v>
-      </c>
-      <c r="F13">
+        <v>3.5187187656249994E-2</v>
+      </c>
+      <c r="F19">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
         <v>37</v>
       </c>
-      <c r="F15" t="s">
+      <c r="F21" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
         <v>21</v>
       </c>
-      <c r="B16">
+      <c r="B22">
         <v>3000</v>
       </c>
-      <c r="D16">
-        <f>B16/100</f>
+      <c r="D22">
+        <f>B22/100</f>
         <v>30</v>
       </c>
-      <c r="F16">
-        <f>B16/4.29</f>
+      <c r="F22">
+        <f>B22/4.29</f>
         <v>699.30069930069931</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
         <v>20</v>
       </c>
-      <c r="B17">
+      <c r="B23">
         <v>1050</v>
       </c>
-      <c r="C17">
+      <c r="C23">
         <v>3000</v>
       </c>
-      <c r="D17">
-        <f t="shared" ref="D17:E21" si="3">B17/100</f>
+      <c r="D23">
+        <f t="shared" ref="D23:E27" si="3">B23/100</f>
         <v>10.5</v>
       </c>
-      <c r="E17">
+      <c r="E23">
         <f t="shared" si="3"/>
         <v>30</v>
       </c>
-      <c r="F17">
-        <f t="shared" ref="F17:F21" si="4">B17/4.29</f>
+      <c r="F23">
+        <f t="shared" ref="F23:F27" si="4">B23/4.29</f>
         <v>244.75524475524475</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
         <v>19</v>
       </c>
-      <c r="B18">
+      <c r="B24">
         <v>300</v>
       </c>
-      <c r="C18">
+      <c r="C24">
         <v>1050</v>
       </c>
-      <c r="D18">
+      <c r="D24">
         <f t="shared" si="3"/>
         <v>3</v>
       </c>
-      <c r="E18">
+      <c r="E24">
         <f t="shared" si="3"/>
         <v>10.5</v>
       </c>
-      <c r="F18">
+      <c r="F24">
         <f t="shared" si="4"/>
         <v>69.930069930069934</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
         <v>22</v>
       </c>
-      <c r="B19">
+      <c r="B25">
         <v>150</v>
       </c>
-      <c r="C19">
+      <c r="C25">
         <v>300</v>
       </c>
-      <c r="D19">
+      <c r="D25">
         <f t="shared" si="3"/>
         <v>1.5</v>
       </c>
-      <c r="E19">
+      <c r="E25">
         <f t="shared" si="3"/>
         <v>3</v>
       </c>
-      <c r="F19">
+      <c r="F25">
         <f t="shared" si="4"/>
         <v>34.965034965034967</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
         <v>30</v>
       </c>
-      <c r="B20">
+      <c r="B26">
         <v>75</v>
       </c>
-      <c r="C20">
+      <c r="C26">
         <v>150</v>
       </c>
-      <c r="D20">
+      <c r="D26">
         <f t="shared" si="3"/>
         <v>0.75</v>
       </c>
-      <c r="E20">
+      <c r="E26">
         <f t="shared" si="3"/>
         <v>1.5</v>
       </c>
-      <c r="F20">
+      <c r="F26">
         <f t="shared" si="4"/>
         <v>17.482517482517483</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
         <v>31</v>
       </c>
-      <c r="B21">
+      <c r="B27">
         <v>0</v>
       </c>
-      <c r="C21">
+      <c r="C27">
         <v>75</v>
       </c>
-      <c r="D21">
+      <c r="D27">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="E21">
+      <c r="E27">
         <f t="shared" si="3"/>
         <v>0.75</v>
       </c>
-      <c r="F21">
+      <c r="F27">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>27</v>
-      </c>
-      <c r="B23" t="s">
-        <v>35</v>
-      </c>
-      <c r="C23" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>28</v>
-      </c>
-      <c r="D24">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>29</v>
-      </c>
-      <c r="D25">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>44</v>
-      </c>
-      <c r="D27">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>39</v>
-      </c>
-      <c r="D28">
-        <v>250</v>
-      </c>
-      <c r="E28">
-        <v>350</v>
-      </c>
-    </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>40</v>
-      </c>
-      <c r="D29">
-        <v>150</v>
-      </c>
-      <c r="E29">
-        <v>250</v>
+        <v>27</v>
+      </c>
+      <c r="B29" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C29" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>41</v>
+        <v>28</v>
       </c>
       <c r="D30">
-        <v>55</v>
-      </c>
-      <c r="E30">
-        <v>150</v>
+        <v>35</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>42</v>
+        <v>29</v>
       </c>
       <c r="D31">
-        <v>35</v>
-      </c>
-      <c r="E31">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>43</v>
-      </c>
-      <c r="D32">
         <v>12</v>
-      </c>
-      <c r="E32">
-        <v>35</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>22</v>
+        <v>44</v>
       </c>
       <c r="D33">
-        <v>0</v>
-      </c>
-      <c r="E33">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>39</v>
+      </c>
+      <c r="D34">
+        <v>250</v>
+      </c>
+      <c r="E34">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>40</v>
+      </c>
+      <c r="D35">
+        <v>150</v>
+      </c>
+      <c r="E35">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>41</v>
+      </c>
+      <c r="D36">
+        <v>55</v>
+      </c>
+      <c r="E36">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>42</v>
+      </c>
+      <c r="D37">
+        <v>35</v>
+      </c>
+      <c r="E37">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>43</v>
+      </c>
+      <c r="D38">
         <v>12</v>
+      </c>
+      <c r="E38">
+        <v>35</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
+        <v>22</v>
+      </c>
+      <c r="D39">
+        <v>0</v>
+      </c>
+      <c r="E39">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
         <v>33</v>
       </c>
-      <c r="B39" t="s">
+      <c r="B45" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
         <v>36</v>
       </c>
-      <c r="D40">
+      <c r="D46">
         <v>25</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
         <v>29</v>
       </c>
-      <c r="D41">
+      <c r="D47">
         <v>10</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B29" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>